<commit_message>
add spring MVC send data between view and controller
</commit_message>
<xml_diff>
--- a/Utils_Hien/Spring_send data View _Controller.xlsx
+++ b/Utils_Hien/Spring_send data View _Controller.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>Send data from view to controller</t>
   </si>
@@ -85,9 +85,6 @@
     <t>JSP file</t>
   </si>
   <si>
-    <t>Controller</t>
-  </si>
-  <si>
     <t>@RequestMapping(value = "/login", method = RequestMethod.POST)</t>
   </si>
   <si>
@@ -128,15 +125,80 @@
   </si>
   <si>
     <t>User user = userService.authenticated(u.getUsername(), u.getPassword());</t>
+  </si>
+  <si>
+    <t>2. use form</t>
+  </si>
+  <si>
+    <t>jsp file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;form action='calculation' method='post'&gt; </t>
+  </si>
+  <si>
+    <t>&lt;/form&gt;</t>
+  </si>
+  <si>
+    <t>Controller Handle</t>
+  </si>
+  <si>
+    <t>1. requestparam</t>
+  </si>
+  <si>
+    <t>2. ModelAttribute</t>
+  </si>
+  <si>
+    <t>@Pathvariable</t>
+  </si>
+  <si>
+    <t>com.demo.test.Model</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>com.demo.test.Domain</t>
+  </si>
+  <si>
+    <t>-&gt; database</t>
+  </si>
+  <si>
+    <t>-&gt; view</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>name, pass, product</t>
+  </si>
+  <si>
+    <t>name, pass</t>
+  </si>
+  <si>
+    <t>abc.com?name=a&amp;pass=b&amp;product=a</t>
+  </si>
+  <si>
+    <t>abc.com/?/</t>
+  </si>
+  <si>
+    <t>3. PathVariable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,12 +231,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -196,16 +263,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -214,8 +281,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="1162050"/>
-          <a:ext cx="5648325" cy="4657725"/>
+          <a:off x="514350" y="1209676"/>
+          <a:ext cx="5648325" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -253,13 +320,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -308,14 +375,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -324,8 +391,63 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10629900" y="5857874"/>
-          <a:ext cx="7734300" cy="3457575"/>
+          <a:off x="10629900" y="6886575"/>
+          <a:ext cx="7734300" cy="2981326"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10934700" y="1228725"/>
+          <a:ext cx="2943225" cy="981075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -649,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V48"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,256 +782,333 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="R6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="S10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F20" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E24" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F25" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D27" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S30" s="1" t="s">
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C32" s="1" t="s">
+      <c r="S37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S32" s="1" t="s">
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T33" s="1" t="s">
+      <c r="T38" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U39" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C34" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G35" s="1" t="s">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U35" s="1" t="s">
+      <c r="U40" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D37" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D38" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U38" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="E39" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U39" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="E40" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U40" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U42" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V41" s="1" t="s">
+      <c r="V45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V46" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="E42" s="1" t="s">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="V42" s="1" t="s">
+      <c r="V48" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D43" s="1" t="s">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U49" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U43" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="D44" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V44" s="1" t="s">
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U50" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="U45" s="1" t="s">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="T51" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U46" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="T48" s="1" t="s">
-        <v>17</v>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O55" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F56" s="1">
+        <v>2</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O56" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add file validate spring with resource bundle
</commit_message>
<xml_diff>
--- a/Utils_Hien/Spring_send data View _Controller.xlsx
+++ b/Utils_Hien/Spring_send data View _Controller.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
   <si>
     <t>Send data from view to controller</t>
   </si>
@@ -182,6 +182,87 @@
   </si>
   <si>
     <t>3. PathVariable</t>
+  </si>
+  <si>
+    <t>4. getParametter</t>
+  </si>
+  <si>
+    <t>3. use href</t>
+  </si>
+  <si>
+    <t>&lt;a href="./salary?idEm=${item.getEmployeeID()}"&gt;Salary Calculate&lt;/a&gt;&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:forEach var="item" items="${listEmployee}"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td style="width: 15% !important;  word-break: break-all;"&gt;${item.getIdEml()}&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td style="width: 30% !important; word-break: break-all;"&gt;${item.getFirstname()}&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td style="width: 25% !important; word-break: break-all;"&gt;${item.getLastname()}&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td style="width: 20% !important; word-break: break-all;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/tr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/c:forEach&gt;</t>
+  </si>
+  <si>
+    <t>@RequestMapping(value = "/addCustomer", method = RequestMethod.POST)</t>
+  </si>
+  <si>
+    <t>public String addCustomer(Model mm, HttpServletRequest req) {</t>
+  </si>
+  <si>
+    <t>String name = req.getParameter("name");</t>
+  </si>
+  <si>
+    <t>String age = req.getParameter("age");</t>
+  </si>
+  <si>
+    <t>mm.addAttribute("name", name);</t>
+  </si>
+  <si>
+    <t>mm.addAttribute("age", age);</t>
+  </si>
+  <si>
+    <t>return "showinfo";</t>
+  </si>
+  <si>
+    <t>@RequestMapping(value = "/{number}/{name}", method = RequestMethod.GET)</t>
+  </si>
+  <si>
+    <t>public String home2(Model model, @PathVariable String number, @PathVariable String name) {</t>
+  </si>
+  <si>
+    <t>model.addAttribute("number", number);</t>
+  </si>
+  <si>
+    <t>model.addAttribute("name", name);</t>
+  </si>
+  <si>
+    <t>return "home";</t>
+  </si>
+  <si>
+    <t>5. Object (Spring MVC)</t>
+  </si>
+  <si>
+    <t>public String addCustomer(Model mm, Customer customer) {</t>
+  </si>
+  <si>
+    <t>mm.addAttribute("name", customer.getName());</t>
+  </si>
+  <si>
+    <t>mm.addAttribute("age", customer.getAge());</t>
   </si>
 </sst>
 </file>
@@ -428,13 +509,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -448,6 +529,281 @@
         <a:xfrm>
           <a:off x="10934700" y="1228725"/>
           <a:ext cx="2943225" cy="981075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10944225" y="1276350"/>
+          <a:ext cx="6715125" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="2514600"/>
+          <a:ext cx="4657725" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10315575" y="11391901"/>
+          <a:ext cx="5095876" cy="2228850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485774" y="11420475"/>
+          <a:ext cx="7820025" cy="1762125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="476250" y="14697076"/>
+          <a:ext cx="7820025" cy="1314450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -771,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V59"/>
+  <dimension ref="A1:V83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,81 +1138,114 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="L4" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="S4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1109,6 +1498,102 @@
     <row r="59" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T65" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D67" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T67" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T68" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T69" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="S70" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C79" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D80" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>